<commit_message>
Backup for both testcases
</commit_message>
<xml_diff>
--- a/src/test/java/com/ErosNow/testData/LoginData1.xlsx
+++ b/src/test/java/com/ErosNow/testData/LoginData1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neha\eclipse-workspace\ErosNow\src\test\java\com\ErosNow\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB680F9-01F4-4D53-A457-CE2AA3B4A7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395EFE1D-7F78-43CC-8924-AED18093CFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B0379AC4-7BD5-4C7B-B029-425CBB0A4A1A}"/>
   </bookViews>
@@ -60,15 +60,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -82,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,18 +90,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2184A9E8-CC8F-47CA-85D9-3CBB88FDB63F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,15 +444,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>9594505207</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -443,19 +460,15 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>9820347924</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>